<commit_message>
changing in excel file
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kafeel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kafeel\Desktop\lateef\code_playground\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EC06899-9A05-4730-A9DD-3698B9FE1498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAA98A2-C9FB-4ADA-A452-908E041889F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{193E1EF1-03D0-48CC-AFF0-2DCD0617040C}"/>
   </bookViews>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -396,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90CC2188-3848-45BB-A397-1F138CD0AA1F}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -426,6 +415,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>